<commit_message>
update test_data files for regression tests
'Harmonized-DB' --> 'Harmonized'
</commit_message>
<xml_diff>
--- a/tests/test_data/test_global_only.xlsx
+++ b/tests/test_data/test_global_only.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kikstra\Documents\GitHub\aneris\tests\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B8AD68-A13D-46BB-941A-76732EB70104}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4725" yWindow="3705" windowWidth="18675" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -46,23 +52,23 @@
     <t>World</t>
   </si>
   <si>
-    <t>prefix|Emissions|BC|Harmonized-DB</t>
-  </si>
-  <si>
-    <t>prefix|Emissions|Sulfur|Harmonized-DB</t>
-  </si>
-  <si>
     <t>Mt BC/yr</t>
   </si>
   <si>
     <t>Mt SO2/yr</t>
+  </si>
+  <si>
+    <t>prefix|Emissions|BC|Harmonized</t>
+  </si>
+  <si>
+    <t>prefix|Emissions|Sulfur|Harmonized</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +131,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -171,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,9 +217,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,6 +269,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,14 +462,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -453,19 +508,19 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>30</v>
       </c>
       <c r="G2">
-        <v>34.28571428571428</v>
+        <v>34.285714285714278</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -476,16 +531,16 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
       <c r="F3">
         <v>15</v>
       </c>
       <c r="G3">
-        <v>17.14285714285715</v>
+        <v>17.142857142857149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests: Update regression tests baseline for actual base_year
</commit_message>
<xml_diff>
--- a/tests/test_data/test_global_only.xlsx
+++ b/tests/test_data/test_global_only.xlsx
@@ -462,7 +462,7 @@
         <v>30</v>
       </c>
       <c r="G2">
-        <v>34.28571428571428</v>
+        <v>34.66666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -485,7 +485,7 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>17.14285714285715</v>
+        <v>17.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
harmonize: Use partial to reduce explicit method list (#27)
* Bring back stickler's flake8 configuration

The flake8 invoked by stickler seems to ignore setup.cfg.

* _io: Use yaml.safe_load

* harmonize: Use partial to reduce explicit method list

* harmonize: Pass harmonize_year to harmonization methods

Fixes #28.

* tests: Update regression tests baseline for actual base_year
</commit_message>
<xml_diff>
--- a/tests/test_data/test_global_only.xlsx
+++ b/tests/test_data/test_global_only.xlsx
@@ -462,7 +462,7 @@
         <v>30</v>
       </c>
       <c r="G2">
-        <v>34.28571428571428</v>
+        <v>34.66666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -485,7 +485,7 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>17.14285714285715</v>
+        <v>17.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>